<commit_message>
Updated script with a CSV dump. Added experimental script for SharePoint authentication.
</commit_message>
<xml_diff>
--- a/Master_Spreadsheet.xlsx
+++ b/Master_Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14808\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\School\Fall 2020\IFT 402\ASEULA\ASEULA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869BF175-7961-4B7B-A25A-08F78BDAE24E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12C0883-07EE-4505-9A6F-4A4714B8823D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{C3E34DE6-4361-424D-84E5-1C6227D1DF66}"/>
+    <workbookView minimized="1" xWindow="2460" yWindow="2460" windowWidth="21600" windowHeight="11505" activeTab="4" xr2:uid="{C3E34DE6-4361-424D-84E5-1C6227D1DF66}"/>
   </bookViews>
   <sheets>
     <sheet name="20200721 Complete Listing" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16342" uniqueCount="2908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16348" uniqueCount="2911">
   <si>
     <t>sites/Fulton/ETS/sysmgmt/software/Lists/Software</t>
   </si>
@@ -9067,6 +9067,15 @@
   </si>
   <si>
     <t>Updated master spreadsheet.</t>
+  </si>
+  <si>
+    <t>Experimented with SharePlum and Office365 REST API packages for SharePoint user authentication.</t>
+  </si>
+  <si>
+    <t>Developed a function to dump results from script to a CSV file.</t>
+  </si>
+  <si>
+    <t>Researched web and application framework to determine steps for future GUI.</t>
   </si>
 </sst>
 </file>
@@ -94038,7 +94047,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAEA874-8B24-402C-A6B9-BA1C05EAE6E9}">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A78" sqref="A78"/>
@@ -94888,25 +94897,58 @@
         <v>2814</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="78" t="s">
+    <row r="77" spans="1:5" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="73" t="s">
+        <v>2910</v>
+      </c>
+      <c r="B77" s="74">
+        <v>44047</v>
+      </c>
+      <c r="C77" s="72" t="s">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="73" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B78" s="74">
+        <v>44048</v>
+      </c>
+      <c r="C78" s="72" t="s">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="73" t="s">
+        <v>2909</v>
+      </c>
+      <c r="B79" s="74">
+        <v>44048</v>
+      </c>
+      <c r="C79" s="72" t="s">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="78" t="s">
         <v>2906</v>
       </c>
-      <c r="B77" s="69" t="s">
+      <c r="B80" s="69" t="s">
         <v>2837</v>
       </c>
-      <c r="C77" s="69" t="s">
+      <c r="C80" s="69" t="s">
         <v>2837</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="73" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="73" t="s">
         <v>2907</v>
       </c>
-      <c r="B78" s="74">
+      <c r="B81" s="74">
         <v>44045</v>
       </c>
-      <c r="C78" s="72" t="s">
+      <c r="C81" s="72" t="s">
         <v>2814</v>
       </c>
     </row>

</xml_diff>